<commit_message>
VN02 Site list change
</commit_message>
<xml_diff>
--- a/vSmart/Ver 1.2/Policy_Matrix.xlsx
+++ b/vSmart/Ver 1.2/Policy_Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python\L-Oreal\vSmart\Ver 1.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E46DDBB2-1666-45C8-9EDA-F1F685B10CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBD2B2B2-C9D3-4CA8-9719-EF1A8BAA536E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,24 +30,13 @@
     <sheet name="Color-list" sheetId="15" r:id="rId15"/>
     <sheet name="Site-list" sheetId="16" r:id="rId16"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
   <fileRecoveryPr repairLoad="1"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10190" uniqueCount="1601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10190" uniqueCount="1598">
   <si>
     <t>Site Name</t>
   </si>
@@ -5640,6 +5629,10 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">   site-id 20843302
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">   site-id 20912253
 </t>
   </si>
@@ -5664,27 +5657,43 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">  site-list sl_CN20_HKGW_TEST
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  site-list sl_JP01
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 22222288
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20622304
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20862324
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">   site-id 28523311
 </t>
   </si>
   <si>
-    <t xml:space="preserve">  site-list sl_CN20_HKGW_TEST
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  site-list sl_JP01
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 22222288
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20622304
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20862324
+    <t xml:space="preserve">  site-list sl_CloudonRamp_Meraki_VPN2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20622306
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20862331
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20622301
 </t>
   </si>
   <si>
@@ -5692,19 +5701,23 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">  site-list sl_CloudonRamp_Meraki_VPN2
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20622306
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20862331
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20622301
+    <t xml:space="preserve">   site-id 22222299
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  site-list sl_ID04
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  site-list JP02_1000eye
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20642101-20642102
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20862332
 </t>
   </si>
   <si>
@@ -5712,23 +5725,27 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">   site-id 22222299
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  site-list sl_ID04
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  site-list JP02_1000eye
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20642101-20642102
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20862332
+    <t xml:space="preserve">  site-list sl_CN25_HKGW_TEST
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20622104
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  site-list sl_SGDC
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 22222233
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20643303
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20862333-20862334
 </t>
   </si>
   <si>
@@ -5736,30 +5753,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">  site-list sl_CN25_HKGW_TEST
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20622104
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  site-list sl_SGDC
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 22222233
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20643303
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20862333-20862334
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">   site-id 20861114
 </t>
   </si>
@@ -5772,15 +5765,35 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">   site-id 20862312-20862314
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  site-list sl_INDIA_Sites
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  site-list JP07_1000eye_VPN2_Zscaler
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20652301
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20862341
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">  site-list sl_ASIA_SOUTH_Sites
 </t>
   </si>
   <si>
-    <t xml:space="preserve">   site-id 20862312-20862314
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  site-list sl_INDIA_Sites
+    <t xml:space="preserve">   site-id 20910201-20910299
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  site-list sl_SHGW
 </t>
   </si>
   <si>
@@ -5788,23 +5801,23 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">  site-list JP07_1000eye_VPN2_Zscaler
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20652301
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20862341
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20910201-20910299
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  site-list sl_SHGW
+    <t xml:space="preserve">   site-id 22222222
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20652305
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20862351
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  site-list sl_DP_CHINA_IGW_TEST
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20911103-20911133
 </t>
   </si>
   <si>
@@ -5812,26 +5825,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">   site-id 22222222
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20652305
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20862351
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  site-list sl_DP_CHINA_IGW_TEST
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20911103-20911133
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">   site-id 20653201-20653299
 </t>
   </si>
@@ -5844,31 +5837,51 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">  site-list NozScaler_sites
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20653308
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20862408
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20862409
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20912207-20912209
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  site-list sl_dp_India_Sites
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">  site-list sl_dp_South_Asia_Sites
 </t>
   </si>
   <si>
-    <t xml:space="preserve">  site-list NozScaler_sites
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20653308
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20862408
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20862409
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20912207-20912209
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  site-list sl_dp_India_Sites
+    <t xml:space="preserve">   site-id 20612103-20612199
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20662302
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20862417
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20912211
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20910238
 </t>
   </si>
   <si>
@@ -5876,23 +5889,19 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">   site-id 20612103-20612199
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20662302
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20862417
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20912211
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20910238
+    <t xml:space="preserve">   site-id 20822101
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20862410
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20912214
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20910255
 </t>
   </si>
   <si>
@@ -5900,19 +5909,23 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">   site-id 20822101
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20862410
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20912214
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20910255
+    <t xml:space="preserve">   site-id 20822103-20822104
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20862412
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  site-list sl_CN40
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20912216
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20911133
 </t>
   </si>
   <si>
@@ -5920,23 +5933,15 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">   site-id 20822103-20822104
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20862412
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  site-list sl_CN40
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20912216
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20911133
+    <t xml:space="preserve">   site-id 20822107-20822199
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20822101-20822104
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20912218
 </t>
   </si>
   <si>
@@ -5944,15 +5949,11 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">   site-id 20822107-20822199
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20822101-20822104
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20912218
+    <t xml:space="preserve">   site-id 20822106-20822199
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20912223
 </t>
   </si>
   <si>
@@ -5960,11 +5961,23 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">   site-id 20822106-20822199
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20912223
+    <t xml:space="preserve">  site-list TH01_DNS_61
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  site-list sl_AAR_SAAS
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20662301-20662302
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  site-list sl_CN50
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20912226
 </t>
   </si>
   <si>
@@ -5972,23 +5985,11 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">  site-list TH01_DNS_61
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  site-list sl_AAR_SAAS
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20662301-20662302
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  site-list sl_CN50
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20912226
+    <t xml:space="preserve">   site-id 20662222
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20912229
 </t>
   </si>
   <si>
@@ -5996,11 +5997,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">   site-id 20662222
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20912229
+    <t xml:space="preserve">   site-id 20912231
 </t>
   </si>
   <si>
@@ -6008,7 +6005,15 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">   site-id 20912231
+    <t xml:space="preserve">  site-list TW01_DNS_1000eye
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  site-list sl_COR_DP_Intra_DNS_North_Zscale
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20912232
 </t>
   </si>
   <si>
@@ -6016,18 +6021,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">  site-list TW01_DNS_1000eye
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  site-list sl_COR_DP_Intra_DNS_North_Zscale
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20912232
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">   site-id 22222266
 </t>
   </si>
@@ -6108,23 +6101,31 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">   site-id 22222255
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20666222
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20912358
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">   site-id 20642101
 </t>
   </si>
   <si>
-    <t xml:space="preserve">   site-id 22222255
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20843302
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20666222
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20912358
+    <t xml:space="preserve">   site-id 20913157
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  site-list sl_DP_CN40
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   site-id 20912430
 </t>
   </si>
   <si>
@@ -6132,18 +6133,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">   site-id 20913157
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  site-list sl_DP_CN40
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   site-id 20912430
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">   site-id 28803101
 </t>
   </si>
@@ -6187,20 +6176,6 @@
   </si>
   <si>
     <t>Column3</t>
-  </si>
-  <si>
-    <t>_vpn2_dp_India_Sites_VPN2_vpn1_dp_India_Sites_VPN1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">     destination-data-prefix-list dpl_MSTeams_TCP_PREFIXES
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">     destination-data-prefix-list dpl_DNS
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -6253,16 +6228,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6282,13 +6254,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="SL_Matrix" displayName="SL_Matrix" ref="A1:AX108">
-  <autoFilter ref="A1:AX108" xr:uid="{00000000-0009-0000-0100-000001000000}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="VN02"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AX108" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="50">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Site Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ALL-SITES"/>
@@ -6440,14 +6406,7 @@
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="site-name" displayName="site_name" ref="A1:D108">
-  <autoFilter ref="A1:D108" xr:uid="{00000000-0009-0000-0100-000003000000}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="VN01"/>
-        <filter val="VN02"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:D108" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Site Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Policy 1"/>
@@ -6463,16 +6422,8 @@
   <autoFilter ref="A1:F108" xr:uid="{00000000-0009-0000-0100-000004000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="PH01"/>
-        <filter val="PH04"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="1">
-      <filters>
-        <filter val="cp_FROM_ASIA_North_Subzone"/>
-        <filter val="cp_FROM_ASIA_South_Subzone"/>
-        <filter val="cp_FROM_CHINA_Subzone"/>
-        <filter val="cp_FROM_INDIA_Subzone"/>
+        <filter val="VN01"/>
+        <filter val="VN02"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -6896,9 +6847,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AX108"/>
   <sheetViews>
-    <sheetView topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AO131" sqref="AO131"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -7095,7 +7044,7 @@
         <v>1597</v>
       </c>
     </row>
-    <row r="2" spans="1:50" hidden="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -7109,7 +7058,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:50" hidden="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -7123,7 +7072,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:50" hidden="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>50</v>
       </c>
@@ -7137,7 +7086,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:50" hidden="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -7151,7 +7100,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:50" hidden="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -7165,7 +7114,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:50" hidden="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -7179,7 +7128,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:50" hidden="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -7193,7 +7142,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:50" hidden="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -7207,7 +7156,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:50" hidden="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -7221,7 +7170,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:50" hidden="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -7235,7 +7184,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:50" hidden="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -7249,7 +7198,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:50" hidden="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -7263,7 +7212,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:50" hidden="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -7277,7 +7226,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:50" hidden="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -7291,7 +7240,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:50" hidden="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -7305,7 +7254,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -7319,7 +7268,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>64</v>
       </c>
@@ -7333,7 +7282,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -7347,7 +7296,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>66</v>
       </c>
@@ -7361,7 +7310,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -7375,7 +7324,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>68</v>
       </c>
@@ -7383,7 +7332,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>69</v>
       </c>
@@ -7397,7 +7346,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>70</v>
       </c>
@@ -7411,7 +7360,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -7425,7 +7374,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>72</v>
       </c>
@@ -7433,7 +7382,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>73</v>
       </c>
@@ -7447,7 +7396,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>74</v>
       </c>
@@ -7461,7 +7410,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>75</v>
       </c>
@@ -7475,7 +7424,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>76</v>
       </c>
@@ -7489,7 +7438,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>77</v>
       </c>
@@ -7503,7 +7452,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>78</v>
       </c>
@@ -7517,7 +7466,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>79</v>
       </c>
@@ -7531,7 +7480,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>80</v>
       </c>
@@ -7545,7 +7494,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>81</v>
       </c>
@@ -7559,7 +7508,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>82</v>
       </c>
@@ -7573,7 +7522,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>83</v>
       </c>
@@ -7587,7 +7536,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>84</v>
       </c>
@@ -7601,21 +7550,21 @@
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:47" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>85</v>
       </c>
       <c r="N39" t="s">
         <v>48</v>
       </c>
-      <c r="Q39" t="s">
+      <c r="P39" t="s">
         <v>48</v>
       </c>
-      <c r="AU39" t="s">
+      <c r="AT39" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>86</v>
       </c>
@@ -7626,7 +7575,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>87</v>
       </c>
@@ -7640,7 +7589,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>88</v>
       </c>
@@ -7654,7 +7603,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>89</v>
       </c>
@@ -7668,7 +7617,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
         <v>90</v>
       </c>
@@ -7682,7 +7631,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>91</v>
       </c>
@@ -7696,7 +7645,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>92</v>
       </c>
@@ -7710,7 +7659,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>93</v>
       </c>
@@ -7724,7 +7673,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:47" hidden="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
         <v>94</v>
       </c>
@@ -7738,7 +7687,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:34" hidden="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
         <v>95</v>
       </c>
@@ -7752,7 +7701,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:34" hidden="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>96</v>
       </c>
@@ -7766,7 +7715,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:34" hidden="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
         <v>97</v>
       </c>
@@ -7780,7 +7729,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:34" hidden="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
         <v>98</v>
       </c>
@@ -7794,7 +7743,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:34" hidden="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
         <v>99</v>
       </c>
@@ -7808,7 +7757,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="1:34" hidden="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
         <v>100</v>
       </c>
@@ -7822,7 +7771,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="55" spans="1:34" hidden="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
         <v>101</v>
       </c>
@@ -7836,7 +7785,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="1:34" hidden="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
         <v>102</v>
       </c>
@@ -7850,7 +7799,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:34" hidden="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
         <v>103</v>
       </c>
@@ -7864,7 +7813,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:34" hidden="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
         <v>104</v>
       </c>
@@ -7878,7 +7827,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="1:34" hidden="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
         <v>105</v>
       </c>
@@ -7892,7 +7841,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="60" spans="1:34" hidden="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
         <v>106</v>
       </c>
@@ -7906,7 +7855,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="1:34" hidden="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
         <v>107</v>
       </c>
@@ -7920,7 +7869,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="62" spans="1:34" hidden="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
         <v>108</v>
       </c>
@@ -7934,7 +7883,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="63" spans="1:34" hidden="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
         <v>109</v>
       </c>
@@ -7948,7 +7897,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="64" spans="1:34" hidden="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A64" s="2" t="s">
         <v>110</v>
       </c>
@@ -7962,7 +7911,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="65" spans="1:45" hidden="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:45" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
         <v>111</v>
       </c>
@@ -7976,7 +7925,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="66" spans="1:45" hidden="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:45" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
         <v>112</v>
       </c>
@@ -7990,7 +7939,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="67" spans="1:45" hidden="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:45" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
         <v>113</v>
       </c>
@@ -7998,7 +7947,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="68" spans="1:45" hidden="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:45" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
         <v>114</v>
       </c>
@@ -8006,7 +7955,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="69" spans="1:45" hidden="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:45" x14ac:dyDescent="0.15">
       <c r="A69" t="s">
         <v>115</v>
       </c>
@@ -8020,7 +7969,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="70" spans="1:45" hidden="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:45" x14ac:dyDescent="0.15">
       <c r="A70" t="s">
         <v>116</v>
       </c>
@@ -8034,7 +7983,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="71" spans="1:45" hidden="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:45" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
         <v>117</v>
       </c>
@@ -8048,7 +7997,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="72" spans="1:45" hidden="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:45" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
         <v>118</v>
       </c>
@@ -8062,7 +8011,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="73" spans="1:45" hidden="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:45" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
         <v>119</v>
       </c>
@@ -8076,7 +8025,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="74" spans="1:45" hidden="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:45" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
         <v>120</v>
       </c>
@@ -8090,7 +8039,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="75" spans="1:45" hidden="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:45" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
         <v>121</v>
       </c>
@@ -8104,7 +8053,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="76" spans="1:45" hidden="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:45" x14ac:dyDescent="0.15">
       <c r="A76" t="s">
         <v>122</v>
       </c>
@@ -8118,7 +8067,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="77" spans="1:45" hidden="1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:45" x14ac:dyDescent="0.15">
       <c r="A77" t="s">
         <v>123</v>
       </c>
@@ -8132,7 +8081,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="78" spans="1:45" hidden="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:45" x14ac:dyDescent="0.15">
       <c r="A78" t="s">
         <v>124</v>
       </c>
@@ -8146,7 +8095,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="79" spans="1:45" hidden="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:45" x14ac:dyDescent="0.15">
       <c r="A79" t="s">
         <v>125</v>
       </c>
@@ -8160,7 +8109,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="80" spans="1:45" hidden="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:45" x14ac:dyDescent="0.15">
       <c r="A80" t="s">
         <v>126</v>
       </c>
@@ -8174,7 +8123,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="81" spans="1:46" hidden="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A81" t="s">
         <v>127</v>
       </c>
@@ -8188,7 +8137,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="82" spans="1:46" hidden="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
         <v>128</v>
       </c>
@@ -8202,7 +8151,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="83" spans="1:46" hidden="1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
         <v>129</v>
       </c>
@@ -8216,7 +8165,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="84" spans="1:46" hidden="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A84" t="s">
         <v>130</v>
       </c>
@@ -8230,7 +8179,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="85" spans="1:46" hidden="1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
         <v>131</v>
       </c>
@@ -8244,7 +8193,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="86" spans="1:46" hidden="1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A86" t="s">
         <v>132</v>
       </c>
@@ -8258,7 +8207,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="87" spans="1:46" hidden="1" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A87" t="s">
         <v>133</v>
       </c>
@@ -8272,7 +8221,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="88" spans="1:46" hidden="1" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A88" t="s">
         <v>134</v>
       </c>
@@ -8286,7 +8235,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="89" spans="1:46" hidden="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A89" t="s">
         <v>135</v>
       </c>
@@ -8300,7 +8249,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="90" spans="1:46" hidden="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A90" t="s">
         <v>136</v>
       </c>
@@ -8314,7 +8263,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="91" spans="1:46" hidden="1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A91" t="s">
         <v>137</v>
       </c>
@@ -8328,7 +8277,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="92" spans="1:46" hidden="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A92" t="s">
         <v>138</v>
       </c>
@@ -8342,7 +8291,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="93" spans="1:46" hidden="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
         <v>139</v>
       </c>
@@ -8356,7 +8305,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="94" spans="1:46" hidden="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
         <v>140</v>
       </c>
@@ -8370,7 +8319,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="95" spans="1:46" hidden="1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A95" t="s">
         <v>141</v>
       </c>
@@ -8378,7 +8327,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="96" spans="1:46" hidden="1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A96" t="s">
         <v>2</v>
       </c>
@@ -8392,7 +8341,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="97" spans="1:46" hidden="1" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A97" t="s">
         <v>142</v>
       </c>
@@ -8406,7 +8355,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="98" spans="1:46" hidden="1" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A98" t="s">
         <v>143</v>
       </c>
@@ -8414,7 +8363,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="99" spans="1:46" hidden="1" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A99" t="s">
         <v>144</v>
       </c>
@@ -8428,7 +8377,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="100" spans="1:46" hidden="1" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A100" t="s">
         <v>145</v>
       </c>
@@ -8442,7 +8391,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="101" spans="1:46" hidden="1" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A101" t="s">
         <v>146</v>
       </c>
@@ -8456,7 +8405,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="102" spans="1:46" hidden="1" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A102" t="s">
         <v>147</v>
       </c>
@@ -8470,7 +8419,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="103" spans="1:46" hidden="1" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A103" t="s">
         <v>148</v>
       </c>
@@ -8484,7 +8433,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="104" spans="1:46" hidden="1" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A104" s="2" t="s">
         <v>149</v>
       </c>
@@ -8498,7 +8447,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="105" spans="1:46" hidden="1" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A105" t="s">
         <v>150</v>
       </c>
@@ -8506,17 +8455,17 @@
         <v>48</v>
       </c>
     </row>
-    <row r="106" spans="1:46" hidden="1" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A106" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="107" spans="1:46" hidden="1" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A107" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="108" spans="1:46" hidden="1" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A108" t="s">
         <v>153</v>
       </c>
@@ -10946,7 +10895,7 @@
         <v>1383</v>
       </c>
       <c r="E13" t="s">
-        <v>1449</v>
+        <v>1460</v>
       </c>
       <c r="F13" t="s">
         <v>1399</v>
@@ -10955,10 +10904,10 @@
         <v>276</v>
       </c>
       <c r="H13" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="I13" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="J13" t="s">
         <v>276</v>
@@ -10969,19 +10918,19 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="B14" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="C14" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="D14" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="E14" t="s">
-        <v>1466</v>
+        <v>1449</v>
       </c>
       <c r="F14" t="s">
         <v>1380</v>
@@ -11013,7 +10962,7 @@
         <v>1471</v>
       </c>
       <c r="D15" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="E15" t="s">
         <v>1472</v>
@@ -11022,7 +10971,7 @@
         <v>1423</v>
       </c>
       <c r="G15" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="H15" t="s">
         <v>1473</v>
@@ -11034,7 +10983,7 @@
         <v>1396</v>
       </c>
       <c r="K15" t="s">
-        <v>1449</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.15">
@@ -11069,7 +11018,7 @@
         <v>276</v>
       </c>
       <c r="K16" t="s">
-        <v>1466</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.15">
@@ -11121,16 +11070,16 @@
         <v>1474</v>
       </c>
       <c r="E18" t="s">
-        <v>276</v>
+        <v>1490</v>
       </c>
       <c r="F18" t="s">
         <v>1454</v>
       </c>
       <c r="G18" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="H18" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="I18" t="s">
         <v>276</v>
@@ -11150,13 +11099,13 @@
         <v>1404</v>
       </c>
       <c r="C19" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="D19" t="s">
         <v>1376</v>
       </c>
       <c r="E19" t="s">
-        <v>1493</v>
+        <v>276</v>
       </c>
       <c r="F19" t="s">
         <v>1494</v>
@@ -11174,24 +11123,24 @@
         <v>276</v>
       </c>
       <c r="K19" t="s">
-        <v>1496</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B20" t="s">
         <v>1497</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>1498</v>
-      </c>
-      <c r="C20" t="s">
-        <v>1499</v>
       </c>
       <c r="D20" t="s">
         <v>1386</v>
       </c>
       <c r="E20" t="s">
-        <v>1411</v>
+        <v>1499</v>
       </c>
       <c r="F20" t="s">
         <v>1471</v>
@@ -11226,7 +11175,7 @@
         <v>1391</v>
       </c>
       <c r="E21" t="s">
-        <v>1416</v>
+        <v>1411</v>
       </c>
       <c r="F21" t="s">
         <v>1475</v>
@@ -11244,7 +11193,7 @@
         <v>1402</v>
       </c>
       <c r="K21" t="s">
-        <v>276</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.15">
@@ -11252,16 +11201,16 @@
         <v>276</v>
       </c>
       <c r="B22" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="C22" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="D22" t="s">
         <v>1481</v>
       </c>
       <c r="E22" t="s">
-        <v>1422</v>
+        <v>1416</v>
       </c>
       <c r="F22" t="s">
         <v>1489</v>
@@ -11273,13 +11222,13 @@
         <v>1374</v>
       </c>
       <c r="I22" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="J22" t="s">
         <v>276</v>
       </c>
       <c r="K22" t="s">
-        <v>1511</v>
+        <v>276</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.15">
@@ -11296,10 +11245,10 @@
         <v>1488</v>
       </c>
       <c r="E23" t="s">
-        <v>1430</v>
+        <v>1422</v>
       </c>
       <c r="F23" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="G23" t="s">
         <v>1515</v>
@@ -11331,10 +11280,10 @@
         <v>1404</v>
       </c>
       <c r="E24" t="s">
-        <v>1438</v>
+        <v>1430</v>
       </c>
       <c r="F24" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="G24" t="s">
         <v>1521</v>
@@ -11363,10 +11312,10 @@
         <v>1526</v>
       </c>
       <c r="D25" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="E25" t="s">
-        <v>1373</v>
+        <v>1438</v>
       </c>
       <c r="F25" t="s">
         <v>1505</v>
@@ -11401,7 +11350,7 @@
         <v>1504</v>
       </c>
       <c r="E26" t="s">
-        <v>1453</v>
+        <v>1373</v>
       </c>
       <c r="F26" t="s">
         <v>1514</v>
@@ -11433,10 +11382,10 @@
         <v>1426</v>
       </c>
       <c r="D27" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="E27" t="s">
-        <v>1383</v>
+        <v>1453</v>
       </c>
       <c r="F27" t="s">
         <v>1526</v>
@@ -11451,7 +11400,7 @@
         <v>1538</v>
       </c>
       <c r="J27" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="K27" t="s">
         <v>1539</v>
@@ -11471,7 +11420,7 @@
         <v>1513</v>
       </c>
       <c r="E28" t="s">
-        <v>1465</v>
+        <v>1383</v>
       </c>
       <c r="F28" t="s">
         <v>1531</v>
@@ -11506,7 +11455,7 @@
         <v>1545</v>
       </c>
       <c r="E29" t="s">
-        <v>1463</v>
+        <v>1466</v>
       </c>
       <c r="F29" t="s">
         <v>1418</v>
@@ -11535,13 +11484,13 @@
         <v>1446</v>
       </c>
       <c r="C30" t="s">
-        <v>1518</v>
+        <v>1524</v>
       </c>
       <c r="D30" t="s">
         <v>1397</v>
       </c>
       <c r="E30" t="s">
-        <v>1476</v>
+        <v>1464</v>
       </c>
       <c r="F30" t="s">
         <v>1426</v>
@@ -11570,13 +11519,13 @@
         <v>1455</v>
       </c>
       <c r="C31" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="D31" t="s">
         <v>1401</v>
       </c>
       <c r="E31" t="s">
-        <v>1470</v>
+        <v>1476</v>
       </c>
       <c r="F31" t="s">
         <v>1434</v>
@@ -11585,7 +11534,7 @@
         <v>276</v>
       </c>
       <c r="H31" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="I31" t="s">
         <v>1552</v>
@@ -11611,7 +11560,7 @@
         <v>1412</v>
       </c>
       <c r="E32" t="s">
-        <v>1474</v>
+        <v>1470</v>
       </c>
       <c r="F32" t="s">
         <v>276</v>
@@ -11620,7 +11569,7 @@
         <v>1555</v>
       </c>
       <c r="H32" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="I32" t="s">
         <v>1556</v>
@@ -11629,15 +11578,15 @@
         <v>1538</v>
       </c>
       <c r="K32" t="s">
-        <v>1438</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="B33" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="C33" t="s">
         <v>1376</v>
@@ -11646,25 +11595,25 @@
         <v>1417</v>
       </c>
       <c r="E33" t="s">
-        <v>1481</v>
+        <v>1474</v>
       </c>
       <c r="F33" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="G33" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="H33" t="s">
         <v>1505</v>
       </c>
       <c r="I33" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="J33" t="s">
         <v>1541</v>
       </c>
       <c r="K33" t="s">
-        <v>1453</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.15">
@@ -11672,7 +11621,7 @@
         <v>276</v>
       </c>
       <c r="B34" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="C34" t="s">
         <v>1386</v>
@@ -11681,33 +11630,33 @@
         <v>1424</v>
       </c>
       <c r="E34" t="s">
-        <v>1488</v>
+        <v>1481</v>
       </c>
       <c r="F34" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="G34" t="s">
         <v>276</v>
       </c>
       <c r="H34" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="I34" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="J34" t="s">
         <v>1547</v>
       </c>
       <c r="K34" t="s">
-        <v>1465</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="B35" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="C35" t="s">
         <v>1391</v>
@@ -11716,60 +11665,60 @@
         <v>1432</v>
       </c>
       <c r="E35" t="s">
-        <v>1404</v>
+        <v>1488</v>
       </c>
       <c r="F35" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="G35" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="H35" t="s">
         <v>1514</v>
       </c>
       <c r="I35" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="J35" t="s">
         <v>1550</v>
       </c>
       <c r="K35" t="s">
-        <v>1476</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
       <c r="B36" t="s">
         <v>1418</v>
       </c>
       <c r="C36" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="D36" t="s">
         <v>1440</v>
       </c>
       <c r="E36" t="s">
-        <v>1498</v>
+        <v>1404</v>
       </c>
       <c r="F36" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="G36" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="H36" t="s">
         <v>1526</v>
       </c>
       <c r="I36" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="J36" t="s">
         <v>1552</v>
       </c>
       <c r="K36" t="s">
-        <v>1470</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.15">
@@ -11786,7 +11735,7 @@
         <v>1446</v>
       </c>
       <c r="E37" t="s">
-        <v>1504</v>
+        <v>1497</v>
       </c>
       <c r="F37" t="s">
         <v>276</v>
@@ -11798,18 +11747,18 @@
         <v>1531</v>
       </c>
       <c r="I37" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="J37" t="s">
         <v>1556</v>
       </c>
       <c r="K37" t="s">
-        <v>1474</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
       <c r="B38" t="s">
         <v>1500</v>
@@ -11821,25 +11770,25 @@
         <v>1455</v>
       </c>
       <c r="E38" t="s">
-        <v>1508</v>
+        <v>1504</v>
       </c>
       <c r="F38" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="G38" t="s">
-        <v>1575</v>
+        <v>1576</v>
       </c>
       <c r="H38" t="s">
         <v>1426</v>
       </c>
       <c r="I38" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
       <c r="J38" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="K38" t="s">
-        <v>1577</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.15">
@@ -11847,34 +11796,34 @@
         <v>1578</v>
       </c>
       <c r="B39" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="C39" t="s">
         <v>1417</v>
       </c>
       <c r="D39" t="s">
+        <v>1460</v>
+      </c>
+      <c r="E39" t="s">
+        <v>1509</v>
+      </c>
+      <c r="F39" t="s">
+        <v>1491</v>
+      </c>
+      <c r="G39" t="s">
         <v>1579</v>
       </c>
-      <c r="E39" t="s">
-        <v>1513</v>
-      </c>
-      <c r="F39" t="s">
-        <v>1490</v>
-      </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
+        <v>276</v>
+      </c>
+      <c r="I39" t="s">
         <v>1580</v>
       </c>
-      <c r="H39" t="s">
-        <v>276</v>
-      </c>
-      <c r="I39" t="s">
+      <c r="J39" t="s">
+        <v>1567</v>
+      </c>
+      <c r="K39" t="s">
         <v>1581</v>
-      </c>
-      <c r="J39" t="s">
-        <v>1566</v>
-      </c>
-      <c r="K39" t="s">
-        <v>1582</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.15">
@@ -11882,7 +11831,7 @@
         <v>276</v>
       </c>
       <c r="B40" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="C40" t="s">
         <v>1444</v>
@@ -11891,7 +11840,7 @@
         <v>1500</v>
       </c>
       <c r="E40" t="s">
-        <v>1545</v>
+        <v>1513</v>
       </c>
       <c r="F40" t="s">
         <v>1384</v>
@@ -11900,16 +11849,16 @@
         <v>276</v>
       </c>
       <c r="H40" t="s">
+        <v>1583</v>
+      </c>
+      <c r="I40" t="s">
         <v>1584</v>
       </c>
-      <c r="I40" t="s">
+      <c r="J40" t="s">
+        <v>1572</v>
+      </c>
+      <c r="K40" t="s">
         <v>1585</v>
-      </c>
-      <c r="J40" t="s">
-        <v>1571</v>
-      </c>
-      <c r="K40" t="s">
-        <v>1488</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.15">
@@ -11917,13 +11866,13 @@
         <v>1586</v>
       </c>
       <c r="C41" t="s">
-        <v>1579</v>
+        <v>1460</v>
       </c>
       <c r="D41" t="s">
         <v>1507</v>
       </c>
       <c r="E41" t="s">
-        <v>1397</v>
+        <v>1545</v>
       </c>
       <c r="F41" t="s">
         <v>1410</v>
@@ -11935,10 +11884,10 @@
         <v>1587</v>
       </c>
       <c r="J41" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="K41" t="s">
-        <v>1498</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.15">
@@ -11949,10 +11898,10 @@
         <v>1507</v>
       </c>
       <c r="D42" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="E42" t="s">
-        <v>1579</v>
+        <v>1397</v>
       </c>
       <c r="F42" t="s">
         <v>1445</v>
@@ -11961,13 +11910,13 @@
         <v>276</v>
       </c>
       <c r="I42" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="J42" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
       <c r="K42" t="s">
-        <v>1504</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.15">
@@ -11975,7 +11924,7 @@
         <v>276</v>
       </c>
       <c r="C43" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="D43" t="s">
         <v>1516</v>
@@ -11984,16 +11933,16 @@
         <v>1588</v>
       </c>
       <c r="F43" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="I43" t="s">
         <v>1589</v>
       </c>
       <c r="J43" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="K43" t="s">
-        <v>1590</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.15">
@@ -12013,10 +11962,10 @@
         <v>1586</v>
       </c>
       <c r="J44" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="K44" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.15">
@@ -12027,7 +11976,7 @@
         <v>1527</v>
       </c>
       <c r="F45" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="I45" t="s">
         <v>276</v>
@@ -12036,7 +11985,7 @@
         <v>1587</v>
       </c>
       <c r="K45" t="s">
-        <v>1513</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.15">
@@ -12050,10 +11999,10 @@
         <v>1515</v>
       </c>
       <c r="J46" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="K46" t="s">
-        <v>1568</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.15">
@@ -12070,7 +12019,7 @@
         <v>1592</v>
       </c>
       <c r="K47" t="s">
-        <v>1520</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.15">
@@ -12087,7 +12036,7 @@
         <v>1593</v>
       </c>
       <c r="K48" t="s">
-        <v>1579</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="49" spans="3:11" x14ac:dyDescent="0.15">
@@ -12136,63 +12085,63 @@
         <v>1556</v>
       </c>
       <c r="D53" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="54" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C54" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="D54" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="55" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C55" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="D55" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="56" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C56" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="D56" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="57" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C57" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="D57" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="58" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C58" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
       <c r="D58" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="59" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C59" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="D59" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="60" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C60" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="D60" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="61" spans="3:11" x14ac:dyDescent="0.15">
@@ -12208,7 +12157,7 @@
         <v>1589</v>
       </c>
       <c r="D62" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="63" spans="3:11" x14ac:dyDescent="0.15">
@@ -12221,7 +12170,7 @@
     </row>
     <row r="64" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C64" t="s">
-        <v>1466</v>
+        <v>1472</v>
       </c>
       <c r="D64" t="s">
         <v>1449</v>
@@ -12229,15 +12178,15 @@
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.15">
       <c r="C65" t="s">
+        <v>1477</v>
+      </c>
+      <c r="D65" t="s">
         <v>1472</v>
-      </c>
-      <c r="D65" t="s">
-        <v>1466</v>
       </c>
     </row>
     <row r="66" spans="3:4" x14ac:dyDescent="0.15">
       <c r="C66" t="s">
-        <v>1477</v>
+        <v>1483</v>
       </c>
       <c r="D66" t="s">
         <v>1594</v>
@@ -12245,10 +12194,10 @@
     </row>
     <row r="67" spans="3:4" x14ac:dyDescent="0.15">
       <c r="C67" t="s">
-        <v>1483</v>
+        <v>1490</v>
       </c>
       <c r="D67" t="s">
-        <v>1472</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="68" spans="3:4" x14ac:dyDescent="0.15">
@@ -12256,12 +12205,12 @@
         <v>276</v>
       </c>
       <c r="D68" t="s">
-        <v>1477</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="69" spans="3:4" x14ac:dyDescent="0.15">
       <c r="D69" t="s">
-        <v>1483</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="70" spans="3:4" x14ac:dyDescent="0.15">
@@ -12282,9 +12231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -12895,9 +12842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D108"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F126" sqref="F126"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -12919,7 +12864,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -12933,7 +12878,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -12947,7 +12892,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>50</v>
       </c>
@@ -12961,7 +12906,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -12975,7 +12920,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -12989,7 +12934,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -13003,7 +12948,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -13017,7 +12962,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -13031,7 +12976,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -13045,7 +12990,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -13059,7 +13004,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -13073,7 +13018,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -13087,7 +13032,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -13101,7 +13046,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -13115,7 +13060,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -13129,7 +13074,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -13143,7 +13088,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>64</v>
       </c>
@@ -13157,7 +13102,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -13171,7 +13116,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>66</v>
       </c>
@@ -13185,7 +13130,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -13199,7 +13144,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>68</v>
       </c>
@@ -13207,7 +13152,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>69</v>
       </c>
@@ -13221,7 +13166,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>70</v>
       </c>
@@ -13235,7 +13180,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -13249,7 +13194,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>72</v>
       </c>
@@ -13257,7 +13202,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>73</v>
       </c>
@@ -13271,7 +13216,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>74</v>
       </c>
@@ -13285,7 +13230,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>75</v>
       </c>
@@ -13299,7 +13244,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>76</v>
       </c>
@@ -13313,7 +13258,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>77</v>
       </c>
@@ -13327,7 +13272,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>78</v>
       </c>
@@ -13341,7 +13286,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>79</v>
       </c>
@@ -13355,7 +13300,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>80</v>
       </c>
@@ -13369,7 +13314,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>81</v>
       </c>
@@ -13383,7 +13328,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>82</v>
       </c>
@@ -13397,7 +13342,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>83</v>
       </c>
@@ -13433,13 +13378,13 @@
         <v>13</v>
       </c>
       <c r="C39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D39" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>86</v>
       </c>
@@ -13450,7 +13395,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>87</v>
       </c>
@@ -13464,7 +13409,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>88</v>
       </c>
@@ -13478,7 +13423,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>89</v>
       </c>
@@ -13492,7 +13437,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
         <v>90</v>
       </c>
@@ -13506,7 +13451,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>91</v>
       </c>
@@ -13520,7 +13465,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>92</v>
       </c>
@@ -13534,7 +13479,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>93</v>
       </c>
@@ -13548,7 +13493,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
         <v>94</v>
       </c>
@@ -13562,7 +13507,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
         <v>95</v>
       </c>
@@ -13576,7 +13521,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>96</v>
       </c>
@@ -13590,7 +13535,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
         <v>97</v>
       </c>
@@ -13604,7 +13549,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
         <v>98</v>
       </c>
@@ -13618,7 +13563,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
         <v>99</v>
       </c>
@@ -13632,7 +13577,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
         <v>100</v>
       </c>
@@ -13646,7 +13591,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
         <v>101</v>
       </c>
@@ -13660,7 +13605,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
         <v>102</v>
       </c>
@@ -13674,7 +13619,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
         <v>103</v>
       </c>
@@ -13688,7 +13633,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
         <v>104</v>
       </c>
@@ -13702,7 +13647,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
         <v>105</v>
       </c>
@@ -13716,7 +13661,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
         <v>106</v>
       </c>
@@ -13730,7 +13675,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
         <v>107</v>
       </c>
@@ -13744,7 +13689,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
         <v>108</v>
       </c>
@@ -13758,7 +13703,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
         <v>109</v>
       </c>
@@ -13772,7 +13717,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
         <v>110</v>
       </c>
@@ -13786,7 +13731,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
         <v>111</v>
       </c>
@@ -13800,7 +13745,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
         <v>112</v>
       </c>
@@ -13814,7 +13759,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
         <v>113</v>
       </c>
@@ -13822,7 +13767,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
         <v>114</v>
       </c>
@@ -13830,7 +13775,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A69" t="s">
         <v>115</v>
       </c>
@@ -13844,7 +13789,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A70" t="s">
         <v>116</v>
       </c>
@@ -13858,7 +13803,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
         <v>117</v>
       </c>
@@ -13872,7 +13817,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
         <v>118</v>
       </c>
@@ -13886,7 +13831,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
         <v>119</v>
       </c>
@@ -13900,7 +13845,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
         <v>120</v>
       </c>
@@ -13914,7 +13859,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
         <v>121</v>
       </c>
@@ -13928,7 +13873,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A76" t="s">
         <v>122</v>
       </c>
@@ -13942,7 +13887,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A77" t="s">
         <v>123</v>
       </c>
@@ -13956,7 +13901,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A78" t="s">
         <v>124</v>
       </c>
@@ -13970,7 +13915,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A79" t="s">
         <v>125</v>
       </c>
@@ -13984,7 +13929,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A80" t="s">
         <v>126</v>
       </c>
@@ -13998,7 +13943,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A81" t="s">
         <v>127</v>
       </c>
@@ -14012,7 +13957,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
         <v>128</v>
       </c>
@@ -14026,7 +13971,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
         <v>129</v>
       </c>
@@ -14040,7 +13985,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A84" t="s">
         <v>130</v>
       </c>
@@ -14054,7 +13999,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
         <v>131</v>
       </c>
@@ -14068,7 +14013,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A86" t="s">
         <v>132</v>
       </c>
@@ -14082,7 +14027,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A87" t="s">
         <v>133</v>
       </c>
@@ -14096,7 +14041,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A88" t="s">
         <v>134</v>
       </c>
@@ -14110,7 +14055,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A89" t="s">
         <v>135</v>
       </c>
@@ -14124,7 +14069,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A90" t="s">
         <v>136</v>
       </c>
@@ -14138,7 +14083,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A91" t="s">
         <v>137</v>
       </c>
@@ -14152,7 +14097,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A92" t="s">
         <v>138</v>
       </c>
@@ -14166,7 +14111,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
         <v>139</v>
       </c>
@@ -14180,7 +14125,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
         <v>140</v>
       </c>
@@ -14194,7 +14139,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A95" t="s">
         <v>141</v>
       </c>
@@ -14202,7 +14147,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A96" t="s">
         <v>2</v>
       </c>
@@ -14216,7 +14161,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A97" t="s">
         <v>142</v>
       </c>
@@ -14230,7 +14175,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A98" t="s">
         <v>143</v>
       </c>
@@ -14238,7 +14183,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A99" t="s">
         <v>144</v>
       </c>
@@ -14252,7 +14197,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A100" t="s">
         <v>145</v>
       </c>
@@ -14266,7 +14211,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A101" t="s">
         <v>146</v>
       </c>
@@ -14280,7 +14225,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A102" t="s">
         <v>147</v>
       </c>
@@ -14294,7 +14239,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A103" t="s">
         <v>148</v>
       </c>
@@ -14308,7 +14253,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A104" t="s">
         <v>149</v>
       </c>
@@ -14322,7 +14267,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A105" t="s">
         <v>150</v>
       </c>
@@ -14330,17 +14275,17 @@
         <v>42</v>
       </c>
     </row>
-    <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A106" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A107" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A108" t="s">
         <v>153</v>
       </c>
@@ -14362,7 +14307,7 @@
   <dimension ref="A1:F108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M137" sqref="M137"/>
+      <selection activeCell="F123" sqref="F123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -14695,7 +14640,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -14715,7 +14660,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>64</v>
       </c>
@@ -15112,7 +15057,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>84</v>
       </c>
@@ -15132,18 +15077,18 @@
         <v>172</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>85</v>
       </c>
       <c r="B39" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C39" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D39" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E39" t="s">
         <v>161</v>
@@ -16063,7 +16008,7 @@
         <v>214</v>
       </c>
       <c r="D85" t="s">
-        <v>1598</v>
+        <v>223</v>
       </c>
       <c r="E85" t="s">
         <v>161</v>
@@ -18120,9 +18065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AH233"/>
   <sheetViews>
-    <sheetView topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AG14" sqref="AG14:AH61"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -19720,7 +19663,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="27" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>367</v>
       </c>
@@ -19784,8 +19727,8 @@
       <c r="U16" t="s">
         <v>360</v>
       </c>
-      <c r="V16" s="4" t="s">
-        <v>1599</v>
+      <c r="V16" t="s">
+        <v>372</v>
       </c>
       <c r="W16" t="s">
         <v>373</v>
@@ -24394,7 +24337,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="64" spans="1:34" ht="27" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
         <v>363</v>
       </c>
@@ -24485,8 +24428,8 @@
       <c r="AG64" t="s">
         <v>370</v>
       </c>
-      <c r="AH64" s="4" t="s">
-        <v>1600</v>
+      <c r="AH64" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="65" spans="1:34" x14ac:dyDescent="0.15">
@@ -31598,9 +31541,8 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
@@ -39177,9 +39119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -40447,9 +40387,8 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>